<commit_message>
fix bug for cal failrate
</commit_message>
<xml_diff>
--- a/max_injection_rate.xlsx
+++ b/max_injection_rate.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>max_injection_rate_10</t>
+          <t>max_injection_rate_5</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>max_injection_rate_20</t>
+          <t>max_injection_rate_10</t>
         </is>
       </c>
     </row>
@@ -460,13 +460,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C2" t="n">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D2" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -474,27 +474,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D3" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>15</v>
       </c>
-      <c r="B4" t="n">
-        <v>130</v>
-      </c>
-      <c r="C4" t="n">
-        <v>155</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>155</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +498,13 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="C5" t="n">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D5" t="n">
-        <v>145</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +512,13 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="C6" t="n">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="D6" t="n">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +526,13 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="C7" t="n">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="D7" t="n">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +540,13 @@
         <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="C8" t="n">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="D8" t="n">
-        <v>175</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +554,13 @@
         <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="C9" t="n">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="D9" t="n">
-        <v>185</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +568,13 @@
         <v>45</v>
       </c>
       <c r="B10" t="n">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C10" t="n">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="D10" t="n">
-        <v>190</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +582,13 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="C11" t="n">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="D11" t="n">
-        <v>190</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +596,13 @@
         <v>55</v>
       </c>
       <c r="B12" t="n">
+        <v>121</v>
+      </c>
+      <c r="C12" t="n">
         <v>125</v>
       </c>
-      <c r="C12" t="n">
-        <v>185</v>
-      </c>
       <c r="D12" t="n">
-        <v>190</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +610,13 @@
         <v>60</v>
       </c>
       <c r="B13" t="n">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="C13" t="n">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="D13" t="n">
-        <v>175</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +624,13 @@
         <v>65</v>
       </c>
       <c r="B14" t="n">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="C14" t="n">
-        <v>195</v>
+        <v>132</v>
       </c>
       <c r="D14" t="n">
-        <v>195</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +638,13 @@
         <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="C15" t="n">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="D15" t="n">
-        <v>190</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +652,13 @@
         <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="C16" t="n">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="D16" t="n">
-        <v>190</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +666,13 @@
         <v>80</v>
       </c>
       <c r="B17" t="n">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="C17" t="n">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="D17" t="n">
-        <v>215</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +680,13 @@
         <v>85</v>
       </c>
       <c r="B18" t="n">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="C18" t="n">
-        <v>215</v>
+        <v>139</v>
       </c>
       <c r="D18" t="n">
-        <v>215</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +694,13 @@
         <v>90</v>
       </c>
       <c r="B19" t="n">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="C19" t="n">
-        <v>235</v>
+        <v>149</v>
       </c>
       <c r="D19" t="n">
-        <v>235</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +708,13 @@
         <v>95</v>
       </c>
       <c r="B20" t="n">
-        <v>205</v>
+        <v>142</v>
       </c>
       <c r="C20" t="n">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="D20" t="n">
-        <v>255</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>